<commit_message>
for one coop tech deployment
</commit_message>
<xml_diff>
--- a/db/uploads/50gacoops.xlsx
+++ b/db/uploads/50gacoops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansellgabrieldelayre/Sites/GA_system/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63769D58-0481-0140-8D1C-7A8B44F433A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B452171-BB08-7248-BF7B-E6F17D540325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8495" uniqueCount="6657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8531" uniqueCount="6685">
   <si>
     <t>NO.</t>
   </si>
@@ -20081,6 +20081,90 @@
   </si>
   <si>
     <t>CNCL</t>
+  </si>
+  <si>
+    <t>BATAAN COOPERATIVE BANK</t>
+  </si>
+  <si>
+    <t>COOPERATIVE BANK OF CAGAYAN</t>
+  </si>
+  <si>
+    <t>COOPERATIVE BANK OF MOUNTAIN PROVINCE</t>
+  </si>
+  <si>
+    <t>COOPERATIVE BANK OF NEGROS ORIENTAL</t>
+  </si>
+  <si>
+    <t>COOPERATIVE BANK OF ZAMBALES</t>
+  </si>
+  <si>
+    <t>METRO SOUTH COOPERATIVE BANK</t>
+  </si>
+  <si>
+    <t>MINDANAO CONSOLIDATED COOPERATIVE BANK</t>
+  </si>
+  <si>
+    <t>NETWORK CONSOLIDATED COOPERATIVE BANK</t>
+  </si>
+  <si>
+    <t>OCCIDENTAL MINDORO COOPERATIVE BANK</t>
+  </si>
+  <si>
+    <t>BANCO COOPERATIVA DE ZAMBOANGA</t>
+  </si>
+  <si>
+    <t>AGA00530</t>
+  </si>
+  <si>
+    <t>AGA00531</t>
+  </si>
+  <si>
+    <t>AGA00532</t>
+  </si>
+  <si>
+    <t>AGA00533</t>
+  </si>
+  <si>
+    <t>AGA00534</t>
+  </si>
+  <si>
+    <t>AGA00535</t>
+  </si>
+  <si>
+    <t>AGA00536</t>
+  </si>
+  <si>
+    <t>AGA00537</t>
+  </si>
+  <si>
+    <t>AGA00538</t>
+  </si>
+  <si>
+    <t>AGA00539</t>
+  </si>
+  <si>
+    <t>AGA00540</t>
+  </si>
+  <si>
+    <t>AGA00541</t>
+  </si>
+  <si>
+    <t>AGA00542</t>
+  </si>
+  <si>
+    <t>AGA00543</t>
+  </si>
+  <si>
+    <t>AGA00544</t>
+  </si>
+  <si>
+    <t>AGA00545</t>
+  </si>
+  <si>
+    <t>AGA00546</t>
+  </si>
+  <si>
+    <t>AGA00547</t>
   </si>
 </sst>
 </file>
@@ -20090,7 +20174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -20242,6 +20326,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -20520,7 +20610,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -20784,6 +20874,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -74669,10 +74760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C528"/>
+  <dimension ref="A2:C545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="102" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A199" sqref="A199"/>
+    <sheetView tabSelected="1" topLeftCell="A514" zoomScale="102" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B528" sqref="B528:B545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -80468,7 +80559,150 @@
         <v>6656</v>
       </c>
     </row>
-    <row r="528" spans="1:3" ht="16" thickTop="1"/>
+    <row r="528" spans="1:3" ht="17" thickTop="1">
+      <c r="A528" s="101" t="s">
+        <v>6657</v>
+      </c>
+      <c r="B528" s="101" t="s">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" ht="16">
+      <c r="A529" s="101" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B529" s="101" t="s">
+        <v>6668</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" ht="16">
+      <c r="A530" s="101" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B530" s="101" t="s">
+        <v>6669</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" ht="16">
+      <c r="A531" s="101" t="s">
+        <v>6658</v>
+      </c>
+      <c r="B531" s="101" t="s">
+        <v>6670</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" ht="16">
+      <c r="A532" s="101" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B532" s="101" t="s">
+        <v>6671</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" ht="16">
+      <c r="A533" s="101" t="s">
+        <v>6659</v>
+      </c>
+      <c r="B533" s="101" t="s">
+        <v>6672</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" ht="16">
+      <c r="A534" s="101" t="s">
+        <v>6660</v>
+      </c>
+      <c r="B534" s="101" t="s">
+        <v>6673</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" ht="16">
+      <c r="A535" s="101" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B535" s="101" t="s">
+        <v>6674</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" ht="16">
+      <c r="A536" s="101" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B536" s="101" t="s">
+        <v>6675</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" ht="16">
+      <c r="A537" s="101" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B537" s="101" t="s">
+        <v>6676</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" ht="16">
+      <c r="A538" s="101" t="s">
+        <v>6661</v>
+      </c>
+      <c r="B538" s="101" t="s">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" ht="16">
+      <c r="A539" s="101" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B539" s="101" t="s">
+        <v>6678</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" ht="16">
+      <c r="A540" s="101" t="s">
+        <v>6662</v>
+      </c>
+      <c r="B540" s="101" t="s">
+        <v>6679</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" ht="16">
+      <c r="A541" s="101" t="s">
+        <v>6663</v>
+      </c>
+      <c r="B541" s="101" t="s">
+        <v>6680</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" ht="16">
+      <c r="A542" s="101" t="s">
+        <v>3478</v>
+      </c>
+      <c r="B542" s="101" t="s">
+        <v>6681</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" ht="16">
+      <c r="A543" s="101" t="s">
+        <v>6664</v>
+      </c>
+      <c r="B543" s="101" t="s">
+        <v>6682</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" ht="16">
+      <c r="A544" s="101" t="s">
+        <v>6665</v>
+      </c>
+      <c r="B544" s="101" t="s">
+        <v>6683</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" ht="16">
+      <c r="A545" s="101" t="s">
+        <v>6666</v>
+      </c>
+      <c r="B545" s="101" t="s">
+        <v>6684</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A527">
     <sortCondition ref="A2:A527"/>

</xml_diff>